<commit_message>
ScorecardKnowledge: update template and import data
</commit_message>
<xml_diff>
--- a/lib/sample/assets/csv/educational_backgrounds.xlsx
+++ b/lib/sample/assets/csv/educational_backgrounds.xlsx
@@ -11,34 +11,128 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>code</t>
   </si>
   <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>ed001</t>
-  </si>
-  <si>
-    <t>bachelor degree</t>
+    <t>name_km</t>
+  </si>
+  <si>
+    <t>name_en</t>
+  </si>
+  <si>
+    <t>edu_001</t>
+  </si>
+  <si>
+    <t>ពុំមានការអប់រំផ្លូវការ</t>
+  </si>
+  <si>
+    <t>No formal school</t>
+  </si>
+  <si>
+    <t>edu_002</t>
+  </si>
+  <si>
+    <t>មិនបញ្ចប់បឋមសិក្សា</t>
+  </si>
+  <si>
+    <t>Incomplete primary</t>
+  </si>
+  <si>
+    <t>edu_003</t>
+  </si>
+  <si>
+    <t>បានបញ្ចប់បឋមសិក្សា</t>
+  </si>
+  <si>
+    <t>Completed primary</t>
+  </si>
+  <si>
+    <t>edu_004</t>
+  </si>
+  <si>
+    <t>មិនបញ្ចប់អនុវិទ្យាល័យ</t>
+  </si>
+  <si>
+    <t>Incomplete lower secondary</t>
+  </si>
+  <si>
+    <t>edu_005</t>
+  </si>
+  <si>
+    <t>បញ្ចប់អនុវិទ្យាល័យ</t>
+  </si>
+  <si>
+    <t>Complete lower secondary</t>
+  </si>
+  <si>
+    <t>edu_006</t>
+  </si>
+  <si>
+    <t>មិនបញ្ចប់វិទ្យាល័យ</t>
+  </si>
+  <si>
+    <t>Incomplete upper secondary</t>
+  </si>
+  <si>
+    <t>edu_007</t>
+  </si>
+  <si>
+    <t>បញ្ចប់វិទ្យាល័យ</t>
+  </si>
+  <si>
+    <t>Complete upper secondary</t>
+  </si>
+  <si>
+    <t>edu_008</t>
+  </si>
+  <si>
+    <t>ខ្ពស់ជាងវិទ្យាល័យ</t>
+  </si>
+  <si>
+    <t>Higher than secondary</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="8">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
-    <font/>
-    <font>
+    <font>
+      <b/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="Battambang"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color theme="1"/>
+      <name val="Battambang"/>
     </font>
   </fonts>
   <fills count="2">
@@ -55,15 +149,30 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -280,21 +389,107 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="2" max="3" width="26.71"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>3</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>